<commit_message>
Supercoach Optimiser  base code working and uploaded to shinyserver
</commit_message>
<xml_diff>
--- a/Data/projections_2021_manual_input.xlsx
+++ b/Data/projections_2021_manual_input.xlsx
@@ -3377,8 +3377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W890"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4958,11 +4958,11 @@
         <v>112</v>
       </c>
       <c r="F23" s="4">
-        <v>-4</v>
+        <v>-10</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H23">
         <v>612554</v>
@@ -24284,11 +24284,11 @@
         <v>68</v>
       </c>
       <c r="F302" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G302" s="2">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H302">
         <v>371667</v>
@@ -26492,11 +26492,11 @@
         <v>65</v>
       </c>
       <c r="F334" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G334" s="2">
         <f t="shared" si="5"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="H334">
         <v>356480</v>
@@ -41699,11 +41699,11 @@
         <v>41</v>
       </c>
       <c r="F554" s="4">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G554" s="2">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="H554">
         <v>224716</v>
@@ -61022,7 +61022,7 @@
         <v>0</v>
       </c>
       <c r="G834" s="2">
-        <f t="shared" ref="G834:G897" si="13">F834+E834</f>
+        <f t="shared" ref="G834:G890" si="13">F834+E834</f>
         <v>1</v>
       </c>
       <c r="H834">

</xml_diff>